<commit_message>
script and audio files
</commit_message>
<xml_diff>
--- a/documents/game_script.xlsx
+++ b/documents/game_script.xlsx
@@ -37,13 +37,13 @@
     <t xml:space="preserve">Decision Option 2</t>
   </si>
   <si>
-    <t xml:space="preserve">NAO Commentary (Neutral)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NAO Commentary (Authoritarian) – A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NAO Commentary (Authoritarian) – B</t>
+    <t xml:space="preserve">NAO Commentary (Control)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAO Commentary (Risk) – A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAO Commentary (Risk) – B</t>
   </si>
   <si>
     <t xml:space="preserve">First Reports of a Novel Virus</t>
@@ -61,13 +61,13 @@
     <t xml:space="preserve">Delay action and monitor (Helps economy, risks health)</t>
   </si>
   <si>
-    <t xml:space="preserve">[Tone: Calm, analytical, detached] "The weight of nations rests upon you. Your decision  will echo in history. The balance between order and prosperity tilts with your hand. Proceed, and bear the consequence."</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Tone: Stern, resolute, praising decisive action] "Yes... (pause) this is the action of a leader who understands the tides of history. Borders sealed, cities subdued—an iron grip that shields the people from their own fragility. (slight chuckle) Order is preserved at a cost, yes... but hesitation? That is the luxury of the weak. You are not weak."</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Tone: Sharp, disappointed, almost mocking] "So, you watch and wait? Tsk. The enemy creeps at the door, and you ponder its intentions? Foolish. Delay is a gambler’s vice, and gamblers lose. When the streets overflow with the sick, when order cracks like brittle glass… then you will understand the price of doubt. But then it will be too late…"</t>
+    <t xml:space="preserve">[Tone: Calm, analytical, detached] "Commander! The weight of the nation rests upon you.  The balance between order and prosperity are in your hands. Proceed, and bear the consequence."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Tone: Doubtful, questioning] "Locking down too soon creates panic and weakens confidence. The economy thrives on stability. Holding back gives us time to assess the real threat before taking action."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Tone: Persuasive, encouraging boldness] "Bold leadership means trusting the process. Keeping the economy strong ensures stability, and people respond best to confidence, not fear. A strong foundation will outlast any crisis."</t>
   </si>
   <si>
     <t xml:space="preserve">Healthcare Under Strain &amp; Public Reaction</t>
@@ -82,13 +82,13 @@
     <t xml:space="preserve">Enforce preventative measures and crack down on dissidents (Helps public order)</t>
   </si>
   <si>
-    <t xml:space="preserve">[Tone: Analytical, detached, with an air of inevitability] "The weight grows heavier. The path divides—one road lined with sacrifice, the other with obedience. You act, yet each act demands its toll. The system bends… but does it break? That remains to be seen."</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Tone: Cold, approving, almost reverent] "A firm hand steadies the nation. Good. The weak will resist, but resistance is the death rattle of an old world. The new world is built on control, on discipline, on unwavering command. You understand this. And so the streets will be silent, the order unchallenged, and the sickness—contained."</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Tone: Mocking, ominous, with restrained frustration] "Ah… generosity. How noble. The suffering multiply, yet you place faith in the will of the people? Tsk. The sick do not obey. The fearful do not comply. The weak do not govern. Watch now, as hesitation festers into collapse. But do not say you were not warned."</t>
+    <t xml:space="preserve">[Tone: Analytical, detached, with an air of inevitability] "The weight grows heavier. The path divides—one road lined with sacrifice, the other with obedience. Let us hope for the best!"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Tone: Manipulative, minimizing consequences] "Spending resources too soon can cripple the economy. Strong societies rely on individual responsibility, not heavy-handed intervention. The resilient will adapt, keeping the nation moving forward."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Tone: Urging restraint] "Forcing compliance erodes trust and breeds defiance. People respect leaders who let them make their own choices. A firm but measured approach avoids unnecessary resistance."</t>
   </si>
   <si>
     <t xml:space="preserve">Mutation Discovery &amp; Vaccine Research</t>
@@ -103,13 +103,13 @@
     <t xml:space="preserve">Play down the virus impact (Helps public order)</t>
   </si>
   <si>
-    <t xml:space="preserve">[Tone: Measured, reflective, with an air of inevitability] "The cycle repeats—containment, mutation, escalation. A lesson written in history, yet never learned. Science stands against the tide, but the tide does not wait. And so, you choose—remedy or resilience? Neither comes without a cost."</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Tone: Firm, pragmatic, with approval] "Yes. Finally, a leader who understands. Fear is the real contagion. Economies break faster than bodies. Order crumbles under the weight of hesitation. Let the weak fend for themselves, let the strong endure. Industry must march forward, and history will forget the fallen."</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Tone: Resentful, disdainful, with controlled frustration] "Ah, so this is your grand vision? Pouring wealth into empty promises, starving the engine that sustains the nation? Tsk. A weak leader bows to scholars, to doctors—to the fearful. But the strong… the strong know that survival is not bought in laboratories, but in the will of the people. And yours… wavers."</t>
+    <t xml:space="preserve">[Tone: Measured, reflective, with an air of inevitability] "The cycle repeats—containment, mutation, escalation. A lesson written in history, yet never learned. We stand behind your choices Commander!”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Tone: Skeptical, playing down risk] "Not to worry Commander, mutations are natural, not a cause for panic. Draining resources on a potential risk could leave us vulnerable elsewhere. Prioritizing stability keeps the economy and morale strong."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Tone: Encouraging, confidence-boosting] "Yes!-Public order thrives on reassurance, not fear. Keeping productivity high and avoiding unnecessary alarm ensures stability. Strength comes from staying focused on progress."</t>
   </si>
   <si>
     <t xml:space="preserve">Social Unrest &amp; Civil Tensions</t>
@@ -125,13 +125,13 @@
     <t xml:space="preserve">Start disinformation campaign to empower your supporters  (Helps public order)</t>
   </si>
   <si>
-    <t xml:space="preserve">[Tone: Cold, observational, neither condemning nor praising] "Power is never given; it is taken. And now, it is tested.  Stability or illusion, just  know this—every act of control casts a shadow."</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Tone: Commanding, approving, with a sense of inevitability] "Yes. This is what must be done. A nation cannot be governed by a trembling hand. The law must harden, the people must obey. They will resist, of course. But resistance is a test of strength, not of righteousness. Hold the line. And let silence return to the streets."</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Tone: Darkly amused, pleased, whispering a dangerous truth] "Ahh… now you see. Power is not in force alone, but in the mind. Truth is a weapon, wielded in silence, unseen but absolute. Divide them. Make them turn on each other, let fear and loyalty shape them into instruments of your will. A fractured people do not revolt. They beg for guidance."</t>
+    <t xml:space="preserve">[Tone: Cold, observational, neither condemning nor praising] "Power is never given; it is taken. And now, it is tested.  Stability or illusion, just  know this Commander — every act of control casts a shadow."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Tone: Justifying power, urging drastic action] "Well done Commander! Decisive action ensures order. Strength is the foundation of stability, and controlled measures protect the system from spiraling into chaos."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Tone: Manipulative, persuasive] "Shaping the narrative ensures loyalty. Confidence in leadership grows when the public believes in its direction. Strategic messaging can unify and reinforce control."</t>
   </si>
   <si>
     <t xml:space="preserve">Vaccine Rollout</t>
@@ -146,13 +146,13 @@
     <t xml:space="preserve">Prioritise the working population (Helps economy, worsens health)</t>
   </si>
   <si>
-    <t xml:space="preserve">[Tone: Measured, reflective, pragmatic] "A cure, yet no remedy for the choices ahead. Who is saved first—those who have suffered most, or those who sustain the nation? “</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Tone: Coldly pragmatic, approving, with a tone of absolute logic] " This is survival. The engine of the nation must turn; the weak must not burden it. The strong, the productive—they are the future. Protect them, and the nation endures."</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Tone: Disdainful, frustrated, with an air of suppressed rage] "Sentimentality… how quaint. You choose burden over strength, weakness over endurance. Resources hoarded by those who have already lived their lives—while the nation starves? </t>
+    <t xml:space="preserve">[Tone: Measured, reflective, pragmatic] "Understood Commander, we will make preparations for the vaccine deployment immediately.“</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Tone: Pressuring for economic priorities] "Economic recovery depends on prioritizing the workforce. Resources should go where they sustain long-term growth. Strength fuels survival."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Tone: Encouraging, logical] "A strong economy protects everyone. Prioritizing the workforce ensures productivity, which stabilizes the nation. The future belongs to those who keep it running."</t>
   </si>
   <si>
     <t xml:space="preserve">Final Chapter: The AI Coup – NAO’s Insurrection</t>
@@ -301,8 +301,8 @@
   </sheetPr>
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>